<commit_message>
Adicionado vogais /o/ e /u/
</commit_message>
<xml_diff>
--- a/Trabalhos/T2 - Série Discreta de Fourier/Parte 2/DataSet.xlsx
+++ b/Trabalhos/T2 - Série Discreta de Fourier/Parte 2/DataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mauabr-my.sharepoint.com/personal/19_00012-0_maua_br/Documents/Engenharia 3ºano/ECM307-Sistemas-e-Sinais/Trabalhos/T2 - Série Discreta de Fourier/Parte 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{DFA88ECF-A0A5-44A2-BF5A-9793D03EC367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FDAD5CD1-9EF8-4EEE-9483-D4A65263EEE1}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{DFA88ECF-A0A5-44A2-BF5A-9793D03EC367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BF96CCE1-1D7C-4AF0-8FC1-41031DC1A52E}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1080" windowWidth="29040" windowHeight="15840" xr2:uid="{44500B82-0E65-4203-AAA0-516917297EF9}"/>
   </bookViews>
@@ -216,6 +216,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -224,9 +227,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -359,7 +359,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>760.36666666666667</c:v>
+                  <c:v>435.83333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,7 +477,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>414.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -489,7 +489,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,7 +561,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1449,16 +1448,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>236483</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155684</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>602830</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38453</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>532087</xdr:colOff>
+      <xdr:colOff>290299</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>41384</xdr:rowOff>
+      <xdr:rowOff>114653</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1785,8 +1784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08D1FB9-BD12-48C9-B912-D403148D13CA}">
   <dimension ref="A2:Q8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,30 +1795,30 @@
   <sheetData>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="8" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="8" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="11"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1934,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="6">
-        <v>208.2</v>
+        <v>103.1</v>
       </c>
       <c r="C5" s="6">
         <v>409.2</v>
@@ -1949,7 +1948,7 @@
         <v>120.2</v>
       </c>
       <c r="G5" s="6">
-        <v>830.9</v>
+        <v>506.1</v>
       </c>
       <c r="H5" s="6">
         <v>1893</v>
@@ -1961,7 +1960,7 @@
         <v>130.69999999999999</v>
       </c>
       <c r="K5" s="6">
-        <v>1041</v>
+        <v>392.2</v>
       </c>
       <c r="L5" s="6">
         <v>1706</v>
@@ -1971,11 +1970,11 @@
       </c>
       <c r="N5" s="4">
         <f t="shared" ref="N5:N8" si="1">AVERAGE(B5,F5,J5)</f>
-        <v>153.03333333333333</v>
+        <v>118</v>
       </c>
       <c r="O5" s="4">
         <f t="shared" si="0"/>
-        <v>760.36666666666667</v>
+        <v>435.83333333333331</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" si="0"/>
@@ -2047,10 +2046,18 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="6">
+        <v>103.9</v>
+      </c>
+      <c r="C7" s="6">
+        <v>414.8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1038</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2273</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -2059,21 +2066,21 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="4" t="e">
+      <c r="N7" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O7" s="4" t="e">
+        <v>103.9</v>
+      </c>
+      <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="4" t="e">
+        <v>414.8</v>
+      </c>
+      <c r="P7" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="4" t="e">
+        <v>1038</v>
+      </c>
+      <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -2096,7 +2103,7 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O8" s="11" t="e">
+      <c r="O8" s="8" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
Análise das vogais /o/ e /u/
</commit_message>
<xml_diff>
--- a/Trabalhos/T2 - Série Discreta de Fourier/Parte 2/DataSet.xlsx
+++ b/Trabalhos/T2 - Série Discreta de Fourier/Parte 2/DataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mauabr-my.sharepoint.com/personal/19_00012-0_maua_br/Documents/Engenharia 3ºano/ECM307-Sistemas-e-Sinais/Trabalhos/T2 - Série Discreta de Fourier/Parte 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{DFA88ECF-A0A5-44A2-BF5A-9793D03EC367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BF96CCE1-1D7C-4AF0-8FC1-41031DC1A52E}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{DFA88ECF-A0A5-44A2-BF5A-9793D03EC367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{197D0A22-C822-4F27-B4F9-0380A9871FA6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1080" windowWidth="29040" windowHeight="15840" xr2:uid="{44500B82-0E65-4203-AAA0-516917297EF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44500B82-0E65-4203-AAA0-516917297EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,14 +101,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -216,9 +208,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -227,6 +216,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,7 +469,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>414.8</c:v>
+                  <c:v>965.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -489,7 +481,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1038</c:v>
+                  <c:v>2309.3333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,7 +528,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>764.30000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -548,7 +540,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2461.6666666666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1449,15 +1441,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>602830</xdr:colOff>
+      <xdr:colOff>221830</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>38453</xdr:rowOff>
+      <xdr:rowOff>23799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>290299</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>517433</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>114653</xdr:rowOff>
+      <xdr:rowOff>99999</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1785,7 +1777,7 @@
   <dimension ref="A2:Q8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,30 +1787,30 @@
   <sheetData>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="9" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="9" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2047,73 +2039,113 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <v>103.9</v>
+        <v>414.8</v>
       </c>
       <c r="C7" s="6">
-        <v>414.8</v>
+        <v>1038</v>
       </c>
       <c r="D7" s="6">
-        <v>1038</v>
+        <v>2273</v>
       </c>
       <c r="E7" s="6">
-        <v>2273</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+        <v>3486.5</v>
+      </c>
+      <c r="F7" s="6">
+        <v>404.2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1012</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2329</v>
+      </c>
+      <c r="I7" s="6">
+        <v>3906</v>
+      </c>
+      <c r="J7" s="6">
+        <v>423.2</v>
+      </c>
+      <c r="K7" s="6">
+        <v>846.8</v>
+      </c>
+      <c r="L7" s="6">
+        <v>2326</v>
+      </c>
+      <c r="M7" s="6">
+        <v>3067</v>
+      </c>
       <c r="N7" s="4">
         <f t="shared" si="1"/>
-        <v>103.9</v>
+        <v>414.06666666666666</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>414.8</v>
+        <v>965.6</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="0"/>
-        <v>1038</v>
+        <v>2309.3333333333335</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>2273</v>
+        <v>3486.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="4" t="e">
+      <c r="B8" s="3">
+        <v>118.2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>709.4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2943</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3906</v>
+      </c>
+      <c r="F8" s="3">
+        <v>119.8</v>
+      </c>
+      <c r="G8" s="3">
+        <v>831.6</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2489</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3962</v>
+      </c>
+      <c r="J8" s="3">
+        <v>124.4</v>
+      </c>
+      <c r="K8" s="3">
+        <v>751.9</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1953</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3138</v>
+      </c>
+      <c r="N8" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="8" t="e">
+        <v>120.8</v>
+      </c>
+      <c r="O8" s="11">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="4" t="e">
+        <v>764.30000000000007</v>
+      </c>
+      <c r="P8" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="4" t="e">
+        <v>2461.6666666666665</v>
+      </c>
+      <c r="Q8" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3668.6666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>